<commit_message>
update media of mediaplayer if listview item is clicked
</commit_message>
<xml_diff>
--- a/mock_data.xlsx
+++ b/mock_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sagar\My Files\vidforge\vid-img-forg-det\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29588AFB-19D5-43E0-B7E3-173F0221C114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E476BB4-1229-43A8-8D13-E066301E0AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -82,6 +82,27 @@
   </si>
   <si>
     <t>Deletion Forgery</t>
+  </si>
+  <si>
+    <t>C:/Users/Sagar/Downloads/vid.mp4</t>
+  </si>
+  <si>
+    <t>C:/Users/Sagar/Downloads/production ID_4713259.mp4</t>
+  </si>
+  <si>
+    <t>C:/Users/Sagar/Downloads/istockphoto.mp4</t>
+  </si>
+  <si>
+    <t>C:/Users/Sagar/Downloads/swan.jpg</t>
+  </si>
+  <si>
+    <t>C:/Users/Sagar/Downloads/scene.jpeg</t>
+  </si>
+  <si>
+    <t>C:/Users/Sagar/Downloads/photo.jpeg</t>
+  </si>
+  <si>
+    <t>C:/Users/Sagar/Downloads/images.jpeg</t>
   </si>
 </sst>
 </file>
@@ -402,7 +423,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,6 +461,9 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -463,6 +487,9 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -486,6 +513,9 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -509,6 +539,9 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -532,6 +565,9 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
@@ -555,6 +591,9 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -577,6 +616,9 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>

</xml_diff>